<commit_message>
Kommentare hinzugefügt, mtt_a hinzugefügt
</commit_message>
<xml_diff>
--- a/Mapping/Mapping_Meta_Py.xlsx
+++ b/Mapping/Mapping_Meta_Py.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Dropbox\ITI\NVT_Data-Model\Mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Administrator/CODE/Github/NVT_Data-Model/Mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C694E5-114E-4488-9EB5-FE0A1F98941F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CD99F5-0988-6546-BC8E-C87467E9CF7B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="2895" windowWidth="24420" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5740" yWindow="480" windowWidth="39680" windowHeight="27340" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produktionen" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="453">
   <si>
     <t>Identifier / geeinigter Name</t>
   </si>
@@ -1303,13 +1303,109 @@
   </si>
   <si>
     <t>nvto:wasIssuedAtTime</t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t>rdfs:label</t>
+  </si>
+  <si>
+    <t>theoretisch als InformationObject möglich</t>
+  </si>
+  <si>
+    <t>(dann mit Agent)</t>
+  </si>
+  <si>
+    <t>mtt_a:gema</t>
+  </si>
+  <si>
+    <t>mtt_a = MTT administrative</t>
+  </si>
+  <si>
+    <t>mtt_a:isDigitised</t>
+  </si>
+  <si>
+    <t>mtt_a:internalLocation</t>
+  </si>
+  <si>
+    <t>mtt_a:visibilityLevel</t>
+  </si>
+  <si>
+    <t>mtt_a:workingComment</t>
+  </si>
+  <si>
+    <t>mtt_a:contentComment</t>
+  </si>
+  <si>
+    <t>nvto:tapeMarkings</t>
+  </si>
+  <si>
+    <t>Tape Markings</t>
+  </si>
+  <si>
+    <t>auch nvto:objectMarkings</t>
+  </si>
+  <si>
+    <t>mtt_a:rightsStatus</t>
+  </si>
+  <si>
+    <t>mtt_a:copiesHeld</t>
+  </si>
+  <si>
+    <t>mtt_a:dateOfLastConditionStatement</t>
+  </si>
+  <si>
+    <t>nvto:objectMarkings</t>
+  </si>
+  <si>
+    <t>Object Markings</t>
+  </si>
+  <si>
+    <t>wenn "Behältnis" eigene Zeile ist (e.g. Mappe)</t>
+  </si>
+  <si>
+    <t>könnte mtt_a: werden</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + nvto:hasDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + rdfs:label</t>
+  </si>
+  <si>
+    <t>nvto:lifetimeExtent</t>
+  </si>
+  <si>
+    <t>auch mtt_a möglich</t>
+  </si>
+  <si>
+    <t>has lifetime with extent of</t>
+  </si>
+  <si>
+    <t>nvto:relatedWebsite</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + dc:identifier / nvto:hasIdentifier</t>
+  </si>
+  <si>
+    <t>dann =nvto:Organization</t>
+  </si>
+  <si>
+    <t>eher rdfs:label</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + nvto:person</t>
+  </si>
+  <si>
+    <t>label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1340,8 +1436,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1370,6 +1473,18 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor rgb="FFFFFF66"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1437,7 +1552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1482,6 +1597,17 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1820,25 +1946,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" style="10" customWidth="1"/>
     <col min="4" max="4" width="31" style="10" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="10"/>
+    <col min="7" max="7" width="11.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37" style="10" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>253</v>
       </c>
@@ -1860,8 +1987,11 @@
       <c r="G1" s="8" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="10" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1870,7 +2000,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1882,36 +2012,57 @@
       <c r="F3" s="12" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="10" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="10" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -1924,7 +2075,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -1937,7 +2088,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -1950,7 +2101,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
@@ -1963,7 +2114,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
@@ -1976,7 +2127,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
@@ -1989,7 +2140,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
@@ -2002,7 +2153,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
@@ -2015,7 +2166,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
@@ -2028,7 +2179,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>15</v>
       </c>
@@ -2041,7 +2192,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
@@ -2054,7 +2205,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>17</v>
       </c>
@@ -2067,7 +2218,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -2080,7 +2231,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
@@ -2093,7 +2244,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>20</v>
       </c>
@@ -2106,7 +2257,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>21</v>
       </c>
@@ -2119,7 +2270,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>22</v>
       </c>
@@ -2132,7 +2283,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>23</v>
       </c>
@@ -2145,7 +2296,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>24</v>
       </c>
@@ -2158,7 +2309,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
@@ -2171,14 +2322,20 @@
         <v>237</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E28" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
@@ -2191,7 +2348,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
@@ -2204,7 +2361,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>29</v>
       </c>
@@ -2217,7 +2374,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>30</v>
       </c>
@@ -2232,7 +2389,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>31</v>
       </c>
@@ -2247,7 +2404,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>32</v>
       </c>
@@ -2260,7 +2417,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>33</v>
       </c>
@@ -2273,7 +2430,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>34</v>
       </c>
@@ -2286,7 +2443,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>250</v>
       </c>
@@ -2304,7 +2461,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>252</v>
       </c>
@@ -2320,7 +2477,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>251</v>
       </c>
@@ -2344,22 +2501,23 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>253</v>
       </c>
@@ -2381,8 +2539,11 @@
       <c r="G1" s="8" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>184</v>
       </c>
@@ -2390,7 +2551,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>185</v>
       </c>
@@ -2400,36 +2561,45 @@
       <c r="F3" s="3" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="21" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>367</v>
+      <c r="E4" s="22" t="s">
+        <v>422</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>368</v>
+        <v>452</v>
       </c>
       <c r="G4" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="21" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>367</v>
+      <c r="E5" s="22" t="s">
+        <v>422</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>368</v>
+        <v>452</v>
       </c>
       <c r="G5" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="21" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>188</v>
       </c>
@@ -2440,7 +2610,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>180</v>
       </c>
@@ -2451,7 +2621,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>181</v>
       </c>
@@ -2462,7 +2632,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>183</v>
       </c>
@@ -2471,6 +2641,9 @@
       </c>
       <c r="F9" s="3" t="s">
         <v>364</v>
+      </c>
+      <c r="H9" t="s">
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -2480,23 +2653,24 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>253</v>
       </c>
@@ -2518,8 +2692,11 @@
       <c r="G1" s="8" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>189</v>
       </c>
@@ -2527,7 +2704,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>190</v>
       </c>
@@ -2537,36 +2714,45 @@
       <c r="F3" s="3" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="21" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>367</v>
+      <c r="E4" s="22" t="s">
+        <v>422</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>368</v>
+        <v>452</v>
       </c>
       <c r="G4" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="21" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>367</v>
+      <c r="E5" s="22" t="s">
+        <v>422</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>368</v>
+        <v>452</v>
       </c>
       <c r="G5" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="21" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>180</v>
       </c>
@@ -2577,7 +2763,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>181</v>
       </c>
@@ -2588,7 +2774,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>183</v>
       </c>
@@ -2598,8 +2784,11 @@
       <c r="F8" s="3" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
     </row>
@@ -2610,23 +2799,24 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:F6"/>
+    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>253</v>
       </c>
@@ -2649,7 +2839,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>172</v>
       </c>
@@ -2657,7 +2847,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>193</v>
       </c>
@@ -2667,18 +2857,21 @@
       <c r="F3" s="3" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="21" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>252</v>
       </c>
@@ -2696,21 +2889,21 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S58" sqref="S58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>253</v>
       </c>
@@ -2733,7 +2926,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>172</v>
       </c>
@@ -2741,7 +2934,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>196</v>
       </c>
@@ -2751,20 +2944,23 @@
       <c r="F3" s="3" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="21" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>197</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>252</v>
       </c>
@@ -2782,23 +2978,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>253</v>
       </c>
@@ -2820,8 +3018,11 @@
       <c r="G1" s="8" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2829,7 +3030,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -2840,7 +3041,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
@@ -2851,17 +3052,17 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -2872,7 +3073,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
@@ -2883,7 +3084,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -2894,7 +3095,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -2905,7 +3106,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -2916,7 +3117,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -2927,7 +3128,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -2938,7 +3139,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -2949,7 +3150,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -2960,7 +3161,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -2971,7 +3172,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2982,7 +3183,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -2993,7 +3194,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -3004,7 +3205,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -3015,7 +3216,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -3026,7 +3227,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -3037,7 +3238,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -3048,7 +3249,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
@@ -3059,7 +3260,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -3070,7 +3271,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
@@ -3081,7 +3282,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -3092,7 +3293,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -3103,7 +3304,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>25</v>
       </c>
@@ -3114,7 +3315,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
@@ -3125,7 +3326,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>42</v>
       </c>
@@ -3136,7 +3337,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
@@ -3147,12 +3348,20 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
@@ -3163,7 +3372,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>44</v>
       </c>
@@ -3177,7 +3386,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>45</v>
       </c>
@@ -3191,7 +3400,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
@@ -3202,7 +3411,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
@@ -3213,7 +3422,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
@@ -3224,7 +3433,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
         <v>252</v>
       </c>
@@ -3238,7 +3447,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
         <v>276</v>
       </c>
@@ -3262,23 +3471,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20:J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>253</v>
       </c>
@@ -3300,18 +3511,35 @@
       <c r="G1" s="8" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E2" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E3" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
@@ -3319,7 +3547,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -3330,22 +3558,40 @@
         <v>279</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="20" t="s">
+        <v>431</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="20" t="s">
+        <v>430</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
@@ -3359,7 +3605,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -3370,7 +3616,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
@@ -3381,7 +3627,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>56</v>
       </c>
@@ -3392,7 +3638,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>57</v>
       </c>
@@ -3403,7 +3649,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -3414,7 +3660,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>59</v>
       </c>
@@ -3425,7 +3671,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
@@ -3436,7 +3682,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
@@ -3447,7 +3693,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>62</v>
       </c>
@@ -3458,7 +3704,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>63</v>
       </c>
@@ -3469,17 +3715,17 @@
         <v>286</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>66</v>
       </c>
@@ -3490,7 +3736,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>67</v>
       </c>
@@ -3501,7 +3747,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>68</v>
       </c>
@@ -3512,7 +3758,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>69</v>
       </c>
@@ -3523,7 +3769,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>70</v>
       </c>
@@ -3534,7 +3780,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>71</v>
       </c>
@@ -3545,7 +3791,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
@@ -3556,7 +3802,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
@@ -3567,7 +3813,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -3578,7 +3824,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>14</v>
       </c>
@@ -3589,7 +3835,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
@@ -3600,7 +3846,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>16</v>
       </c>
@@ -3611,7 +3857,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>73</v>
       </c>
@@ -3622,7 +3868,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
@@ -3633,7 +3879,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>20</v>
       </c>
@@ -3644,7 +3890,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -3655,7 +3901,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>22</v>
       </c>
@@ -3666,7 +3912,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
@@ -3677,7 +3923,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
@@ -3688,7 +3934,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>24</v>
       </c>
@@ -3699,7 +3945,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -3710,7 +3956,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>27</v>
       </c>
@@ -3721,7 +3967,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>74</v>
       </c>
@@ -3732,7 +3978,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>75</v>
       </c>
@@ -3743,12 +3989,20 @@
         <v>298</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E46" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>76</v>
       </c>
@@ -3759,7 +4013,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>77</v>
       </c>
@@ -3770,7 +4024,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>78</v>
       </c>
@@ -3781,7 +4035,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>33</v>
       </c>
@@ -3792,7 +4046,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>34</v>
       </c>
@@ -3803,7 +4057,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>79</v>
       </c>
@@ -3817,7 +4071,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>80</v>
       </c>
@@ -3831,27 +4085,36 @@
         <v>304</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>432</v>
+      </c>
+      <c r="F57" t="s">
+        <v>433</v>
+      </c>
+      <c r="H57" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>85</v>
       </c>
@@ -3865,7 +4128,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>86</v>
       </c>
@@ -3876,22 +4139,23 @@
         <v>306</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C60" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E60" s="10"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>88</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>89</v>
       </c>
@@ -3900,7 +4164,7 @@
       </c>
       <c r="F62" s="3"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>90</v>
       </c>
@@ -3914,7 +4178,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>91</v>
       </c>
@@ -3928,7 +4192,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>92</v>
       </c>
@@ -3942,7 +4206,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>93</v>
       </c>
@@ -3956,12 +4220,18 @@
         <v>311</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E67" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="H67" s="10" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="15" t="s">
         <v>252</v>
       </c>
@@ -3975,7 +4245,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="15" t="s">
         <v>318</v>
       </c>
@@ -3992,7 +4262,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="15" t="s">
         <v>314</v>
       </c>
@@ -4006,7 +4276,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="15" t="s">
         <v>315</v>
       </c>
@@ -4027,23 +4297,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F58" sqref="E2:F58"/>
+    <sheetView topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20:J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>253</v>
       </c>
@@ -4065,18 +4336,35 @@
       <c r="G1" s="8" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E2" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E3" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
@@ -4084,7 +4372,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -4095,22 +4383,40 @@
         <v>279</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="20" t="s">
+        <v>431</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="20" t="s">
+        <v>430</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
@@ -4124,7 +4430,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -4135,7 +4441,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>97</v>
       </c>
@@ -4146,7 +4452,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>56</v>
       </c>
@@ -4157,7 +4463,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>98</v>
       </c>
@@ -4168,7 +4474,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -4179,7 +4485,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>59</v>
       </c>
@@ -4190,7 +4496,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
@@ -4201,7 +4507,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
@@ -4212,7 +4518,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>62</v>
       </c>
@@ -4223,7 +4529,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>63</v>
       </c>
@@ -4234,17 +4540,17 @@
         <v>323</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>99</v>
       </c>
@@ -4255,7 +4561,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>100</v>
       </c>
@@ -4266,7 +4572,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>101</v>
       </c>
@@ -4277,7 +4583,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>102</v>
       </c>
@@ -4288,7 +4594,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>103</v>
       </c>
@@ -4299,7 +4605,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>104</v>
       </c>
@@ -4310,7 +4616,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>105</v>
       </c>
@@ -4321,7 +4627,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>106</v>
       </c>
@@ -4332,7 +4638,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>107</v>
       </c>
@@ -4343,7 +4649,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
@@ -4354,7 +4660,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>108</v>
       </c>
@@ -4365,7 +4671,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>109</v>
       </c>
@@ -4376,7 +4682,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>110</v>
       </c>
@@ -4385,7 +4691,7 @@
       </c>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>111</v>
       </c>
@@ -4394,7 +4700,7 @@
       </c>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>112</v>
       </c>
@@ -4405,7 +4711,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>113</v>
       </c>
@@ -4416,7 +4722,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>114</v>
       </c>
@@ -4427,7 +4733,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>115</v>
       </c>
@@ -4438,7 +4744,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>116</v>
       </c>
@@ -4449,7 +4755,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>117</v>
       </c>
@@ -4460,7 +4766,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>34</v>
       </c>
@@ -4471,7 +4777,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>118</v>
       </c>
@@ -4482,7 +4788,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>119</v>
       </c>
@@ -4493,7 +4799,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>120</v>
       </c>
@@ -4504,7 +4810,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>79</v>
       </c>
@@ -4518,7 +4824,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>85</v>
       </c>
@@ -4532,19 +4838,25 @@
         <v>305</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E48" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="H48" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>122</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>123</v>
       </c>
@@ -4558,24 +4870,27 @@
         <v>304</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>124</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E53" s="20"/>
+      <c r="H53" s="20"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>89</v>
       </c>
@@ -4584,7 +4899,7 @@
       </c>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>90</v>
       </c>
@@ -4598,7 +4913,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>92</v>
       </c>
@@ -4612,7 +4927,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>93</v>
       </c>
@@ -4626,12 +4941,18 @@
         <v>311</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E58" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="H58" s="10" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
         <v>252</v>
       </c>
@@ -4645,7 +4966,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
         <v>318</v>
       </c>
@@ -4662,7 +4983,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
         <v>314</v>
       </c>
@@ -4676,7 +4997,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
         <v>315</v>
       </c>
@@ -4698,23 +5019,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>253</v>
       </c>
@@ -4736,18 +5059,35 @@
       <c r="G1" s="8" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E2" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E3" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
@@ -4755,7 +5095,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -4766,27 +5106,54 @@
         <v>279</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>438</v>
+      </c>
+      <c r="F6" t="s">
+        <v>439</v>
+      </c>
+      <c r="H6" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="20" t="s">
+        <v>431</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="20" t="s">
+        <v>430</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
@@ -4800,7 +5167,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
@@ -4811,7 +5178,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>97</v>
       </c>
@@ -4822,7 +5189,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>56</v>
       </c>
@@ -4833,7 +5200,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>126</v>
       </c>
@@ -4844,7 +5211,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
@@ -4855,7 +5222,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
@@ -4867,7 +5234,7 @@
       </c>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
@@ -4878,7 +5245,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>61</v>
       </c>
@@ -4889,7 +5256,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>127</v>
       </c>
@@ -4900,18 +5267,17 @@
         <v>198</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>129</v>
       </c>
@@ -4922,7 +5288,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>130</v>
       </c>
@@ -4933,7 +5299,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>131</v>
       </c>
@@ -4944,7 +5310,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>132</v>
       </c>
@@ -4955,7 +5321,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>133</v>
       </c>
@@ -4966,7 +5332,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>134</v>
       </c>
@@ -4977,7 +5343,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>135</v>
       </c>
@@ -4988,7 +5354,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>136</v>
       </c>
@@ -5002,7 +5368,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>137</v>
       </c>
@@ -5016,7 +5382,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>138</v>
       </c>
@@ -5030,7 +5396,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>85</v>
       </c>
@@ -5044,7 +5410,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>86</v>
       </c>
@@ -5055,12 +5421,18 @@
         <v>306</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="H34" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>139</v>
       </c>
@@ -5074,7 +5446,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>140</v>
       </c>
@@ -5085,7 +5457,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>141</v>
       </c>
@@ -5099,21 +5471,24 @@
         <v>354</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E38" s="10"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E39" s="20" t="s">
+        <v>437</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>89</v>
       </c>
@@ -5122,7 +5497,7 @@
       </c>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>90</v>
       </c>
@@ -5136,7 +5511,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>92</v>
       </c>
@@ -5150,7 +5525,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>93</v>
       </c>
@@ -5164,12 +5539,20 @@
         <v>311</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E44" s="20" t="s">
+        <v>435</v>
+      </c>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
         <v>252</v>
       </c>
@@ -5183,7 +5566,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
         <v>318</v>
       </c>
@@ -5200,7 +5583,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
         <v>314</v>
       </c>
@@ -5214,7 +5597,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
         <v>315</v>
       </c>
@@ -5235,23 +5618,25 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>253</v>
       </c>
@@ -5273,18 +5658,35 @@
       <c r="G1" s="8" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E2" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E3" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
@@ -5292,7 +5694,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -5303,22 +5705,40 @@
         <v>279</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="20" t="s">
+        <v>431</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="20" t="s">
+        <v>430</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
@@ -5332,7 +5752,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -5343,7 +5763,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>142</v>
       </c>
@@ -5354,7 +5774,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>56</v>
       </c>
@@ -5365,7 +5785,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>143</v>
       </c>
@@ -5376,7 +5796,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -5387,7 +5807,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>59</v>
       </c>
@@ -5398,7 +5818,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
@@ -5409,7 +5829,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
@@ -5420,7 +5840,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>62</v>
       </c>
@@ -5431,7 +5851,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>63</v>
       </c>
@@ -5442,19 +5862,17 @@
         <v>286</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
@@ -5465,7 +5883,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
@@ -5476,7 +5894,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>144</v>
       </c>
@@ -5487,7 +5905,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>145</v>
       </c>
@@ -5498,7 +5916,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>70</v>
       </c>
@@ -5509,12 +5927,20 @@
         <v>322</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E27" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>76</v>
       </c>
@@ -5525,7 +5951,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>77</v>
       </c>
@@ -5536,7 +5962,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>78</v>
       </c>
@@ -5547,7 +5973,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
@@ -5558,7 +5984,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>34</v>
       </c>
@@ -5569,7 +5995,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>146</v>
       </c>
@@ -5583,7 +6009,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>80</v>
       </c>
@@ -5597,22 +6023,23 @@
         <v>304</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E37" s="18"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>85</v>
       </c>
@@ -5625,8 +6052,11 @@
       <c r="F38" s="3" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>86</v>
       </c>
@@ -5637,21 +6067,24 @@
         <v>306</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="3"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E40" s="10"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E41" s="20" t="s">
+        <v>437</v>
+      </c>
+      <c r="H41" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>89</v>
       </c>
@@ -5660,7 +6093,7 @@
       </c>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>90</v>
       </c>
@@ -5674,7 +6107,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>91</v>
       </c>
@@ -5688,7 +6121,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>92</v>
       </c>
@@ -5702,7 +6135,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>93</v>
       </c>
@@ -5716,12 +6149,20 @@
         <v>311</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E47" s="20" t="s">
+        <v>435</v>
+      </c>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
         <v>252</v>
       </c>
@@ -5735,7 +6176,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
         <v>318</v>
       </c>
@@ -5752,7 +6193,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
         <v>314</v>
       </c>
@@ -5766,7 +6207,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
         <v>315</v>
       </c>
@@ -5787,22 +6228,24 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>253</v>
       </c>
@@ -5824,16 +6267,22 @@
       <c r="G1" s="8" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>147</v>
       </c>
       <c r="D2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>148</v>
       </c>
@@ -5843,8 +6292,11 @@
       <c r="F3" s="3" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>149</v>
       </c>
@@ -5855,7 +6307,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>150</v>
       </c>
@@ -5866,17 +6318,17 @@
         <v>358</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>151</v>
       </c>
@@ -5887,7 +6339,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>152</v>
       </c>
@@ -5898,12 +6350,21 @@
         <v>362</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="23" t="s">
+        <v>444</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="H10" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>154</v>
       </c>
@@ -5913,8 +6374,11 @@
       <c r="F11" s="3" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>155</v>
       </c>
@@ -5924,8 +6388,11 @@
       <c r="F12" s="3" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>156</v>
       </c>
@@ -5935,8 +6402,11 @@
       <c r="F13" s="3" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>157</v>
       </c>
@@ -5946,8 +6416,11 @@
       <c r="F14" s="3" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>158</v>
       </c>
@@ -5957,8 +6430,11 @@
       <c r="F15" s="3" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>159</v>
       </c>
@@ -5968,8 +6444,11 @@
       <c r="F16" s="3" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>252</v>
       </c>
@@ -5981,6 +6460,9 @@
       </c>
       <c r="F17" s="3" t="s">
         <v>264</v>
+      </c>
+      <c r="H17" t="s">
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -5990,23 +6472,25 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>253</v>
       </c>
@@ -6028,8 +6512,11 @@
       <c r="G1" s="8" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>160</v>
       </c>
@@ -6037,7 +6524,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>161</v>
       </c>
@@ -6047,8 +6534,11 @@
       <c r="F3" s="3" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>162</v>
       </c>
@@ -6059,17 +6549,25 @@
         <v>368</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>164</v>
       </c>
@@ -6080,7 +6578,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>165</v>
       </c>
@@ -6091,7 +6589,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>166</v>
       </c>
@@ -6102,7 +6600,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>167</v>
       </c>
@@ -6113,7 +6611,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>168</v>
       </c>
@@ -6124,7 +6622,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>157</v>
       </c>
@@ -6134,8 +6632,11 @@
       <c r="F12" s="3" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>169</v>
       </c>
@@ -6145,8 +6646,11 @@
       <c r="F13" s="3" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>170</v>
       </c>
@@ -6156,13 +6660,16 @@
       <c r="F14" s="3" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="H14" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>252</v>
       </c>
@@ -6183,23 +6690,25 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>253</v>
       </c>
@@ -6221,8 +6730,11 @@
       <c r="G1" s="8" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>172</v>
       </c>
@@ -6230,14 +6742,17 @@
         <v>384</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>173</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>174</v>
       </c>
@@ -6247,8 +6762,11 @@
       <c r="F4" s="3" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="21" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>175</v>
       </c>
@@ -6259,19 +6777,29 @@
         <v>368</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>176</v>
       </c>
@@ -6282,7 +6810,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>177</v>
       </c>
@@ -6293,7 +6821,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>178</v>
       </c>
@@ -6304,7 +6832,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>179</v>
       </c>
@@ -6315,7 +6843,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>180</v>
       </c>
@@ -6326,7 +6854,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>181</v>
       </c>
@@ -6337,7 +6865,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>182</v>
       </c>
@@ -6347,8 +6875,11 @@
       <c r="F14" s="3" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>170</v>
       </c>
@@ -6358,8 +6889,11 @@
       <c r="F15" s="3" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>169</v>
       </c>
@@ -6369,8 +6903,11 @@
       <c r="F16" s="3" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>183</v>
       </c>
@@ -6380,8 +6917,11 @@
       <c r="F17" s="3" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>252</v>
       </c>
@@ -6395,14 +6935,14 @@
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>385</v>
       </c>
       <c r="B19" t="s">
         <v>261</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="26" t="s">
         <v>375</v>
       </c>
       <c r="E19" s="19" t="s">
@@ -6410,6 +6950,9 @@
       </c>
       <c r="F19" s="3" t="s">
         <v>377</v>
+      </c>
+      <c r="H19" t="s">
+        <v>449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unnötige Erweiterungen aus Mapping/Mapping_Meta_Py.xlsx entfernt und mtt_a.ttl erstellt
</commit_message>
<xml_diff>
--- a/Mapping/Mapping_Meta_Py.xlsx
+++ b/Mapping/Mapping_Meta_Py.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Administrator/CODE/Github/NVT_Data-Model/Mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CD99F5-0988-6546-BC8E-C87467E9CF7B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54957F7-7CD3-A543-8274-C875D2D10C7D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5740" yWindow="480" windowWidth="39680" windowHeight="27340" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5740" yWindow="480" windowWidth="39680" windowHeight="27340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produktionen" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="450">
   <si>
     <t>Identifier / geeinigter Name</t>
   </si>
@@ -1338,12 +1338,6 @@
     <t>mtt_a:contentComment</t>
   </si>
   <si>
-    <t>nvto:tapeMarkings</t>
-  </si>
-  <si>
-    <t>Tape Markings</t>
-  </si>
-  <si>
     <t>auch nvto:objectMarkings</t>
   </si>
   <si>
@@ -1351,9 +1345,6 @@
   </si>
   <si>
     <t>mtt_a:copiesHeld</t>
-  </si>
-  <si>
-    <t>mtt_a:dateOfLastConditionStatement</t>
   </si>
   <si>
     <t>nvto:objectMarkings</t>
@@ -1948,8 +1939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2562,7 +2553,7 @@
         <v>262</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2573,13 +2564,13 @@
         <v>422</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="G4" t="s">
         <v>389</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -2590,13 +2581,13 @@
         <v>422</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="G5" t="s">
         <v>390</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -2643,7 +2634,7 @@
         <v>364</v>
       </c>
       <c r="H9" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -2715,7 +2706,7 @@
         <v>262</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2726,13 +2717,13 @@
         <v>422</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="G4" t="s">
         <v>389</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -2743,13 +2734,13 @@
         <v>422</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="G5" t="s">
         <v>390</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -2785,7 +2776,7 @@
         <v>364</v>
       </c>
       <c r="H8" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -2858,7 +2849,7 @@
         <v>392</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2891,7 +2882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S58" sqref="S58"/>
     </sheetView>
   </sheetViews>
@@ -2945,7 +2936,7 @@
         <v>392</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -3473,8 +3464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:J21"/>
+    <sheetView topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4105,13 +4096,13 @@
         <v>84</v>
       </c>
       <c r="E57" t="s">
+        <v>435</v>
+      </c>
+      <c r="F57" t="s">
+        <v>436</v>
+      </c>
+      <c r="H57" t="s">
         <v>432</v>
-      </c>
-      <c r="F57" t="s">
-        <v>433</v>
-      </c>
-      <c r="H57" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -4225,7 +4216,7 @@
         <v>94</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="H67" s="10" t="s">
         <v>426</v>
@@ -4299,8 +4290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:J21"/>
+    <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4843,7 +4834,7 @@
         <v>121</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H48" s="20" t="s">
         <v>426</v>
@@ -4946,7 +4937,7 @@
         <v>94</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="H58" s="10" t="s">
         <v>426</v>
@@ -5021,8 +5012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5111,13 +5102,13 @@
         <v>125</v>
       </c>
       <c r="E6" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="F6" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="H6" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -5426,7 +5417,7 @@
         <v>121</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H34" s="20" t="s">
         <v>426</v>
@@ -5481,12 +5472,8 @@
       <c r="A39" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E39" s="20" t="s">
-        <v>437</v>
-      </c>
-      <c r="H39" s="20" t="s">
-        <v>426</v>
-      </c>
+      <c r="E39" s="20"/>
+      <c r="H39" s="20"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
@@ -5544,7 +5531,7 @@
         <v>94</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
@@ -5620,8 +5607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6053,7 +6040,7 @@
         <v>305</v>
       </c>
       <c r="H38" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -6077,12 +6064,8 @@
       <c r="A41" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E41" s="20" t="s">
-        <v>437</v>
-      </c>
-      <c r="H41" s="20" t="s">
-        <v>426</v>
-      </c>
+      <c r="E41" s="20"/>
+      <c r="H41" s="20"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
@@ -6154,7 +6137,7 @@
         <v>94</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
@@ -6231,7 +6214,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6279,7 +6262,7 @@
         <v>366</v>
       </c>
       <c r="H2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -6293,7 +6276,7 @@
         <v>356</v>
       </c>
       <c r="H3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -6355,13 +6338,13 @@
         <v>153</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H10" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -6375,7 +6358,7 @@
         <v>364</v>
       </c>
       <c r="H11" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -6389,7 +6372,7 @@
         <v>364</v>
       </c>
       <c r="H12" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -6403,7 +6386,7 @@
         <v>364</v>
       </c>
       <c r="H13" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -6417,7 +6400,7 @@
         <v>365</v>
       </c>
       <c r="H14" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -6431,7 +6414,7 @@
         <v>365</v>
       </c>
       <c r="H15" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -6445,7 +6428,7 @@
         <v>364</v>
       </c>
       <c r="H16" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -6462,7 +6445,7 @@
         <v>264</v>
       </c>
       <c r="H17" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -6535,7 +6518,7 @@
         <v>262</v>
       </c>
       <c r="H3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -6633,7 +6616,7 @@
         <v>365</v>
       </c>
       <c r="H12" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -6647,7 +6630,7 @@
         <v>364</v>
       </c>
       <c r="H13" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -6661,7 +6644,7 @@
         <v>364</v>
       </c>
       <c r="H14" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -6749,7 +6732,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
       <c r="H3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -6763,7 +6746,7 @@
         <v>262</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -6876,7 +6859,7 @@
         <v>364</v>
       </c>
       <c r="H14" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -6890,7 +6873,7 @@
         <v>364</v>
       </c>
       <c r="H15" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -6904,7 +6887,7 @@
         <v>364</v>
       </c>
       <c r="H16" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -6918,7 +6901,7 @@
         <v>364</v>
       </c>
       <c r="H17" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -6952,7 +6935,7 @@
         <v>377</v>
       </c>
       <c r="H19" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update nvto und meta_py
wo skos:prefLabel auch rdfs:label (überall)
Städte, Länder: kein altlabel mehr. präferierter Name ist Name DE (nur das erste von beiden wird erfasst)
nvto:hasHomepage rdfs:subPropertyOf nvto:hasRelatedWebsite erstmal nur relatedWebsite
nvto:Organization -> rdfs:subClassOf nvto:Agent noch unklar: Trennung zwischen Organisation und PerformingArtsGroup
nvto:Organization statt nvto:PerformingArtsGroup bei "loc ist Institution"
nvto:Person -> rdfs:subClassOf nvto:Agent
nvto:Person statt nvto:Agent bei Personen
nvto:hasLabeling neu (hier für Video, Bild Objekte), überproperty von hasLabelingFront hasLabelingBack
Beschreibung_Quelle: skos:note entfernt, mit nvto:hasDescription ersetzt, bei EV und Pers
nvto:hasComposer rdfs:subPropertyOf nvto:hasMusician
</commit_message>
<xml_diff>
--- a/Mapping/Mapping_Meta_Py.xlsx
+++ b/Mapping/Mapping_Meta_Py.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Dropbox\ITI\NVT_Data-Model\Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB94FA8D-25C8-49FE-B10A-8B3D2A0E0F48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FAD21D-FFF2-4645-9FF3-74145C5508C8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="927" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produktionen" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="444">
   <si>
     <t>Identifier / geeinigter Name</t>
   </si>
@@ -810,9 +810,6 @@
     <t>NVTO Property Label</t>
   </si>
   <si>
-    <t>skos:prefLabel</t>
-  </si>
-  <si>
     <t>nvto:PerformingArtsProduction</t>
   </si>
   <si>
@@ -831,9 +828,6 @@
     <t>preferred label</t>
   </si>
   <si>
-    <t>skos:note</t>
-  </si>
-  <si>
     <t>note</t>
   </si>
   <si>
@@ -1131,18 +1125,12 @@
     <t>has date of death</t>
   </si>
   <si>
-    <t>owl:sameAs</t>
-  </si>
-  <si>
     <t>sameAs</t>
   </si>
   <si>
     <t>homepage</t>
   </si>
   <si>
-    <t>nvto:Agent</t>
-  </si>
-  <si>
     <t>skos:altLabel</t>
   </si>
   <si>
@@ -1227,9 +1215,6 @@
     <t>nvto:Series</t>
   </si>
   <si>
-    <t>nvto:hasTitle;skos:prefLabel</t>
-  </si>
-  <si>
     <t>nvto:hasType</t>
   </si>
   <si>
@@ -1284,18 +1269,12 @@
     <t>nvto:hasRecordist;nvto:hasCreator</t>
   </si>
   <si>
-    <t>skos:prefLabel;nvto:hasName</t>
-  </si>
-  <si>
     <t>nvto:hasFirstName</t>
   </si>
   <si>
     <t>nvto:hasFamilyName</t>
   </si>
   <si>
-    <t>nvto:hasHomepage</t>
-  </si>
-  <si>
     <t>nvto:hasDate</t>
   </si>
   <si>
@@ -1338,58 +1317,61 @@
     <t>mtt_a:contentComment</t>
   </si>
   <si>
-    <t>auch nvto:objectMarkings</t>
-  </si>
-  <si>
     <t>mtt_a:rightsStatus</t>
   </si>
   <si>
     <t>mtt_a:copiesHeld</t>
   </si>
   <si>
-    <t>nvto:objectMarkings</t>
-  </si>
-  <si>
-    <t>Object Markings</t>
-  </si>
-  <si>
     <t>wenn "Behältnis" eigene Zeile ist (e.g. Mappe)</t>
   </si>
   <si>
     <t>könnte mtt_a: werden</t>
   </si>
   <si>
-    <t xml:space="preserve"> + nvto:hasDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + rdfs:label</t>
-  </si>
-  <si>
-    <t>nvto:lifetimeExtent</t>
-  </si>
-  <si>
     <t>auch mtt_a möglich</t>
   </si>
   <si>
     <t>has lifetime with extent of</t>
   </si>
   <si>
-    <t>nvto:relatedWebsite</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + dc:identifier / nvto:hasIdentifier</t>
-  </si>
-  <si>
-    <t>dann =nvto:Organization</t>
-  </si>
-  <si>
-    <t>eher rdfs:label</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + nvto:person</t>
-  </si>
-  <si>
     <t>label</t>
+  </si>
+  <si>
+    <t>owl:sameAs;nvto:hasIdentifier</t>
+  </si>
+  <si>
+    <t>mtt_a:lifetimeExtent</t>
+  </si>
+  <si>
+    <t>nvto:hasRelatedWebsite</t>
+  </si>
+  <si>
+    <t>nvto:Organization</t>
+  </si>
+  <si>
+    <t>skos:prefLabel; rdfs:label</t>
+  </si>
+  <si>
+    <t>skos:prefLabel;rdfs:label</t>
+  </si>
+  <si>
+    <t>nvto:hasTitle;skos:prefLabel;rdfs:label</t>
+  </si>
+  <si>
+    <t>skos:prefLabel;nvto:hasName;rdfs:label</t>
+  </si>
+  <si>
+    <t>nvto:Person</t>
+  </si>
+  <si>
+    <t>Stadtname DE ist präferierter Stadtname</t>
+  </si>
+  <si>
+    <t>nvto:hasLabeling</t>
+  </si>
+  <si>
+    <t>has labeling</t>
   </si>
 </sst>
 </file>
@@ -1435,7 +1417,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1469,12 +1451,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1592,13 +1580,13 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1939,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1949,7 +1937,7 @@
     <col min="2" max="2" width="10.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.140625" style="10" customWidth="1"/>
     <col min="4" max="4" width="31" style="10" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" style="10" customWidth="1"/>
@@ -1961,13 +1949,13 @@
         <v>253</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>254</v>
@@ -1976,10 +1964,10 @@
         <v>255</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1988,7 +1976,7 @@
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1998,13 +1986,10 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="11" t="s">
-        <v>395</v>
+        <v>438</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>198</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2040,7 +2025,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="H6" s="10" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2050,7 +2035,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="H7" s="10" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2060,7 +2045,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="11" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>201</v>
@@ -2073,7 +2058,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="11" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>202</v>
@@ -2320,10 +2305,10 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="10" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2333,7 +2318,7 @@
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="11" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>202</v>
@@ -2439,11 +2424,11 @@
         <v>250</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>242</v>
@@ -2457,12 +2442,12 @@
         <v>252</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="11" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>199</v>
@@ -2473,12 +2458,12 @@
         <v>251</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="11" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>200</v>
@@ -2494,18 +2479,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:H5"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="37.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2513,13 +2498,13 @@
         <v>253</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>254</v>
@@ -2528,10 +2513,10 @@
         <v>255</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2539,7 +2524,7 @@
         <v>184</v>
       </c>
       <c r="D2" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2547,58 +2532,50 @@
         <v>185</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>256</v>
+        <v>437</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>440</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="G3" t="s">
+        <v>385</v>
+      </c>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>422</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="G4" t="s">
-        <v>389</v>
-      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="3"/>
       <c r="H4" s="21" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>422</v>
+      <c r="E5" s="25" t="s">
+        <v>415</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>449</v>
+        <v>431</v>
       </c>
       <c r="G5" t="s">
-        <v>390</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>447</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>188</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2606,10 +2583,10 @@
         <v>180</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2617,10 +2594,10 @@
         <v>181</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2628,13 +2605,10 @@
         <v>183</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>363</v>
+        <v>432</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="H9" t="s">
-        <v>445</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -2646,8 +2620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2655,7 +2629,7 @@
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
@@ -2666,13 +2640,13 @@
         <v>253</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>254</v>
@@ -2681,10 +2655,10 @@
         <v>255</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2692,7 +2666,7 @@
         <v>189</v>
       </c>
       <c r="D2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2700,58 +2674,50 @@
         <v>190</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>256</v>
+        <v>437</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>440</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="G3" t="s">
+        <v>385</v>
+      </c>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>422</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="G4" t="s">
-        <v>389</v>
-      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="3"/>
       <c r="H4" s="21" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>422</v>
+      <c r="E5" s="25" t="s">
+        <v>415</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>449</v>
+        <v>431</v>
       </c>
       <c r="G5" t="s">
-        <v>390</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>447</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>180</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2759,10 +2725,10 @@
         <v>181</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2770,13 +2736,10 @@
         <v>183</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>363</v>
+        <v>432</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="H8" t="s">
-        <v>445</v>
+        <v>361</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2792,8 +2755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2801,7 +2764,7 @@
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.140625" customWidth="1"/>
@@ -2812,13 +2775,13 @@
         <v>253</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>254</v>
@@ -2827,7 +2790,7 @@
         <v>255</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2835,7 +2798,7 @@
         <v>172</v>
       </c>
       <c r="D2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2843,14 +2806,12 @@
         <v>193</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>395</v>
+        <v>438</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>440</v>
-      </c>
+        <v>388</v>
+      </c>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -2867,7 +2828,7 @@
         <v>252</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>199</v>
@@ -2883,14 +2844,14 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S58" sqref="S58"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2899,13 +2860,13 @@
         <v>253</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>254</v>
@@ -2914,7 +2875,7 @@
         <v>255</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2922,7 +2883,7 @@
         <v>172</v>
       </c>
       <c r="D2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2930,14 +2891,12 @@
         <v>196</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>395</v>
+        <v>438</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>440</v>
-      </c>
+        <v>388</v>
+      </c>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -2956,7 +2915,7 @@
         <v>252</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>199</v>
@@ -2971,8 +2930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2981,7 +2940,7 @@
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="8" max="8" width="28.85546875" customWidth="1"/>
@@ -2992,13 +2951,13 @@
         <v>253</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>254</v>
@@ -3007,10 +2966,10 @@
         <v>255</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3018,7 +2977,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3026,10 +2985,10 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>256</v>
+        <v>437</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3037,7 +2996,7 @@
         <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>201</v>
@@ -3058,10 +3017,10 @@
         <v>37</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3069,10 +3028,10 @@
         <v>38</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3080,10 +3039,10 @@
         <v>39</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3091,10 +3050,10 @@
         <v>40</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3102,7 +3061,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>202</v>
@@ -3311,10 +3270,10 @@
         <v>41</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -3322,10 +3281,10 @@
         <v>42</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -3333,7 +3292,7 @@
         <v>27</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>202</v>
@@ -3344,12 +3303,12 @@
         <v>26</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3357,10 +3316,10 @@
         <v>43</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3368,7 +3327,7 @@
         <v>44</v>
       </c>
       <c r="C35" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>244</v>
@@ -3382,7 +3341,7 @@
         <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>246</v>
@@ -3396,10 +3355,10 @@
         <v>32</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3407,10 +3366,10 @@
         <v>33</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3418,10 +3377,10 @@
         <v>34</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3429,30 +3388,30 @@
         <v>252</v>
       </c>
       <c r="B40" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>263</v>
+        <v>393</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B41" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D41" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -3464,8 +3423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3474,7 +3433,7 @@
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="31.28515625" customWidth="1"/>
@@ -3485,13 +3444,13 @@
         <v>253</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>254</v>
@@ -3500,10 +3459,10 @@
         <v>255</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H1" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3511,10 +3470,10 @@
         <v>46</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3522,12 +3481,12 @@
         <v>47</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3535,7 +3494,7 @@
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3543,10 +3502,10 @@
         <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3554,10 +3513,10 @@
         <v>50</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3565,10 +3524,10 @@
         <v>51</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3576,10 +3535,10 @@
         <v>52</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3587,13 +3546,13 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3601,10 +3560,10 @@
         <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3612,10 +3571,10 @@
         <v>55</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -3623,10 +3582,10 @@
         <v>56</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -3634,10 +3593,10 @@
         <v>57</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -3645,10 +3604,10 @@
         <v>58</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -3656,10 +3615,10 @@
         <v>59</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -3667,10 +3626,10 @@
         <v>60</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3678,10 +3637,10 @@
         <v>61</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3689,7 +3648,7 @@
         <v>62</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>395</v>
+        <v>438</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>198</v>
@@ -3700,10 +3659,10 @@
         <v>63</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -3721,10 +3680,10 @@
         <v>66</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3732,10 +3691,10 @@
         <v>67</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3743,10 +3702,10 @@
         <v>68</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3754,10 +3713,10 @@
         <v>69</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -3765,10 +3724,10 @@
         <v>70</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -3776,10 +3735,10 @@
         <v>71</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3952,7 +3911,7 @@
         <v>27</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>202</v>
@@ -3963,10 +3922,10 @@
         <v>74</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3974,10 +3933,10 @@
         <v>75</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3985,12 +3944,12 @@
         <v>26</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="10" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3998,10 +3957,10 @@
         <v>76</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -4009,178 +3968,178 @@
         <v>77</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C52" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C53" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="C57" t="s">
+        <v>312</v>
+      </c>
       <c r="E57" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="F57" t="s">
-        <v>436</v>
-      </c>
-      <c r="H57" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C58" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>86</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C60" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E60" s="10"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>88</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>89</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F62" s="3"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C63" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C64" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -4188,13 +4147,13 @@
         <v>92</v>
       </c>
       <c r="C65" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -4202,13 +4161,13 @@
         <v>93</v>
       </c>
       <c r="C66" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -4216,10 +4175,10 @@
         <v>94</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="H67" s="10" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -4227,10 +4186,10 @@
         <v>252</v>
       </c>
       <c r="B68" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>199</v>
@@ -4238,47 +4197,47 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B69" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C69" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="B70" t="s">
+        <v>260</v>
+      </c>
+      <c r="D70" t="s">
+        <v>317</v>
+      </c>
+      <c r="E70" s="18" t="s">
         <v>314</v>
-      </c>
-      <c r="B70" t="s">
-        <v>261</v>
-      </c>
-      <c r="D70" t="s">
-        <v>319</v>
-      </c>
-      <c r="E70" s="18" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B71" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D71" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -4290,17 +4249,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" customWidth="1"/>
   </cols>
@@ -4310,13 +4270,13 @@
         <v>253</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>254</v>
@@ -4325,10 +4285,10 @@
         <v>255</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -4336,10 +4296,10 @@
         <v>46</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4347,12 +4307,12 @@
         <v>95</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4360,7 +4320,7 @@
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4368,10 +4328,10 @@
         <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4379,10 +4339,10 @@
         <v>50</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4390,10 +4350,10 @@
         <v>96</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4401,10 +4361,10 @@
         <v>52</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4412,13 +4372,13 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4426,10 +4386,10 @@
         <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4437,10 +4397,10 @@
         <v>97</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4448,10 +4408,10 @@
         <v>56</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4459,10 +4419,10 @@
         <v>98</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4470,10 +4430,10 @@
         <v>58</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4481,10 +4441,10 @@
         <v>59</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4492,10 +4452,10 @@
         <v>60</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4503,10 +4463,10 @@
         <v>61</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4514,7 +4474,7 @@
         <v>62</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>395</v>
+        <v>438</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>198</v>
@@ -4525,10 +4485,10 @@
         <v>63</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4546,10 +4506,10 @@
         <v>99</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4557,10 +4517,10 @@
         <v>100</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4568,10 +4528,10 @@
         <v>101</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4579,10 +4539,10 @@
         <v>102</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4601,10 +4561,10 @@
         <v>104</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4612,10 +4572,10 @@
         <v>105</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4623,10 +4583,10 @@
         <v>106</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4634,10 +4594,10 @@
         <v>107</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4645,7 +4605,7 @@
         <v>27</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>202</v>
@@ -4656,10 +4616,10 @@
         <v>108</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -4667,10 +4627,10 @@
         <v>109</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -4678,7 +4638,7 @@
         <v>110</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F34" s="3"/>
     </row>
@@ -4687,7 +4647,7 @@
         <v>111</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F35" s="3"/>
     </row>
@@ -4696,10 +4656,10 @@
         <v>112</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -4707,10 +4667,10 @@
         <v>113</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -4718,10 +4678,10 @@
         <v>114</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -4729,10 +4689,10 @@
         <v>115</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -4740,10 +4700,10 @@
         <v>116</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -4751,10 +4711,10 @@
         <v>117</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -4762,10 +4722,10 @@
         <v>34</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -4773,7 +4733,7 @@
         <v>118</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>201</v>
@@ -4784,7 +4744,7 @@
         <v>119</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>200</v>
@@ -4795,10 +4755,10 @@
         <v>120</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -4806,13 +4766,13 @@
         <v>79</v>
       </c>
       <c r="C46" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -4820,13 +4780,13 @@
         <v>85</v>
       </c>
       <c r="C47" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -4834,10 +4794,10 @@
         <v>121</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="H48" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -4852,13 +4812,13 @@
         <v>123</v>
       </c>
       <c r="C50" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -4886,7 +4846,7 @@
         <v>89</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F54" s="3"/>
     </row>
@@ -4895,13 +4855,13 @@
         <v>90</v>
       </c>
       <c r="C55" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -4909,13 +4869,13 @@
         <v>92</v>
       </c>
       <c r="C56" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -4923,13 +4883,13 @@
         <v>93</v>
       </c>
       <c r="C57" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -4937,10 +4897,10 @@
         <v>94</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -4948,10 +4908,10 @@
         <v>252</v>
       </c>
       <c r="B59" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>199</v>
@@ -4959,47 +4919,47 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B60" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C60" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="B61" t="s">
+        <v>260</v>
+      </c>
+      <c r="D61" t="s">
+        <v>317</v>
+      </c>
+      <c r="E61" s="18" t="s">
         <v>314</v>
-      </c>
-      <c r="B61" t="s">
-        <v>261</v>
-      </c>
-      <c r="D61" t="s">
-        <v>319</v>
-      </c>
-      <c r="E61" s="18" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B62" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D62" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -5012,17 +4972,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="41.7109375" customWidth="1"/>
@@ -5033,13 +4993,13 @@
         <v>253</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>254</v>
@@ -5048,10 +5008,10 @@
         <v>255</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5059,10 +5019,10 @@
         <v>46</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5070,12 +5030,12 @@
         <v>47</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5083,7 +5043,7 @@
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5091,24 +5051,27 @@
         <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="C6" t="s">
+        <v>312</v>
+      </c>
       <c r="E6" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="F6" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="H6" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5116,10 +5079,10 @@
         <v>50</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5127,10 +5090,10 @@
         <v>51</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5138,10 +5101,10 @@
         <v>52</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5149,13 +5112,13 @@
         <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5163,10 +5126,10 @@
         <v>54</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5174,10 +5137,10 @@
         <v>97</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -5185,10 +5148,10 @@
         <v>56</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5196,10 +5159,10 @@
         <v>126</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -5207,10 +5170,10 @@
         <v>58</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5218,10 +5181,10 @@
         <v>59</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -5230,10 +5193,10 @@
         <v>60</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -5241,10 +5204,10 @@
         <v>61</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -5252,7 +5215,7 @@
         <v>127</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>395</v>
+        <v>438</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>198</v>
@@ -5273,10 +5236,10 @@
         <v>129</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -5284,10 +5247,10 @@
         <v>130</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -5295,10 +5258,10 @@
         <v>131</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -5306,10 +5269,10 @@
         <v>132</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -5317,10 +5280,10 @@
         <v>133</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -5328,10 +5291,10 @@
         <v>134</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -5339,10 +5302,10 @@
         <v>135</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -5350,13 +5313,13 @@
         <v>136</v>
       </c>
       <c r="C29" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -5364,13 +5327,13 @@
         <v>137</v>
       </c>
       <c r="C30" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -5378,10 +5341,10 @@
         <v>138</v>
       </c>
       <c r="C31" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>199</v>
@@ -5392,13 +5355,13 @@
         <v>85</v>
       </c>
       <c r="C32" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -5406,10 +5369,10 @@
         <v>86</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -5417,10 +5380,10 @@
         <v>121</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="H34" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -5428,13 +5391,13 @@
         <v>139</v>
       </c>
       <c r="C35" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -5442,10 +5405,10 @@
         <v>140</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -5453,13 +5416,13 @@
         <v>141</v>
       </c>
       <c r="C37" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -5480,7 +5443,7 @@
         <v>89</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F40" s="3"/>
     </row>
@@ -5489,13 +5452,13 @@
         <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -5503,13 +5466,13 @@
         <v>92</v>
       </c>
       <c r="C42" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -5517,13 +5480,13 @@
         <v>93</v>
       </c>
       <c r="C43" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -5531,12 +5494,12 @@
         <v>94</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
       <c r="H44" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -5544,10 +5507,10 @@
         <v>252</v>
       </c>
       <c r="B45" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>199</v>
@@ -5555,47 +5518,47 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B46" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C46" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="B47" t="s">
+        <v>260</v>
+      </c>
+      <c r="D47" t="s">
+        <v>317</v>
+      </c>
+      <c r="E47" s="18" t="s">
         <v>314</v>
-      </c>
-      <c r="B47" t="s">
-        <v>261</v>
-      </c>
-      <c r="D47" t="s">
-        <v>319</v>
-      </c>
-      <c r="E47" s="18" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B48" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D48" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -5607,8 +5570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5617,7 +5580,7 @@
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
     <col min="8" max="8" width="38" customWidth="1"/>
@@ -5628,13 +5591,13 @@
         <v>253</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>254</v>
@@ -5643,10 +5606,10 @@
         <v>255</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5654,10 +5617,10 @@
         <v>46</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5665,12 +5628,12 @@
         <v>47</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5678,7 +5641,7 @@
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5686,10 +5649,10 @@
         <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5697,10 +5660,10 @@
         <v>50</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5708,10 +5671,10 @@
         <v>51</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5719,10 +5682,10 @@
         <v>52</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5730,13 +5693,13 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5744,10 +5707,10 @@
         <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5755,10 +5718,10 @@
         <v>142</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5766,10 +5729,10 @@
         <v>56</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -5777,10 +5740,10 @@
         <v>143</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5788,10 +5751,10 @@
         <v>58</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -5799,10 +5762,10 @@
         <v>59</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5810,10 +5773,10 @@
         <v>60</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -5821,10 +5784,10 @@
         <v>61</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -5832,7 +5795,7 @@
         <v>62</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>395</v>
+        <v>438</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>198</v>
@@ -5843,10 +5806,10 @@
         <v>63</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -5864,10 +5827,10 @@
         <v>68</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -5875,10 +5838,10 @@
         <v>69</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -5886,10 +5849,10 @@
         <v>144</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -5908,10 +5871,10 @@
         <v>70</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -5919,12 +5882,12 @@
         <v>26</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -5932,10 +5895,10 @@
         <v>76</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -5943,10 +5906,10 @@
         <v>77</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -5954,10 +5917,10 @@
         <v>78</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -5965,10 +5928,10 @@
         <v>33</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -5976,10 +5939,10 @@
         <v>34</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -5987,13 +5950,13 @@
         <v>146</v>
       </c>
       <c r="C33" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -6001,13 +5964,13 @@
         <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -6031,16 +5994,16 @@
         <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H38" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -6048,10 +6011,10 @@
         <v>86</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -6072,7 +6035,7 @@
         <v>89</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F42" s="3"/>
     </row>
@@ -6081,13 +6044,13 @@
         <v>90</v>
       </c>
       <c r="C43" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -6095,13 +6058,13 @@
         <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -6109,13 +6072,13 @@
         <v>92</v>
       </c>
       <c r="C45" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -6123,13 +6086,13 @@
         <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -6137,12 +6100,12 @@
         <v>94</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
       <c r="H47" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -6150,10 +6113,10 @@
         <v>252</v>
       </c>
       <c r="B48" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>199</v>
@@ -6161,47 +6124,47 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B49" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C49" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="B50" t="s">
+        <v>260</v>
+      </c>
+      <c r="D50" t="s">
+        <v>317</v>
+      </c>
+      <c r="E50" s="18" t="s">
         <v>314</v>
-      </c>
-      <c r="B50" t="s">
-        <v>261</v>
-      </c>
-      <c r="D50" t="s">
-        <v>319</v>
-      </c>
-      <c r="E50" s="18" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B51" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D51" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -6213,8 +6176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6222,7 +6185,7 @@
     <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
@@ -6233,13 +6196,13 @@
         <v>253</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>254</v>
@@ -6248,10 +6211,10 @@
         <v>255</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -6259,10 +6222,7 @@
         <v>147</v>
       </c>
       <c r="D2" t="s">
-        <v>366</v>
-      </c>
-      <c r="H2" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6270,13 +6230,10 @@
         <v>148</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>414</v>
+        <v>439</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="H3" t="s">
-        <v>440</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -6284,10 +6241,10 @@
         <v>149</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6295,10 +6252,10 @@
         <v>150</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6316,10 +6273,10 @@
         <v>151</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6327,10 +6284,10 @@
         <v>152</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -6338,13 +6295,13 @@
         <v>153</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="H10" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -6352,13 +6309,10 @@
         <v>154</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>363</v>
+        <v>432</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="H11" t="s">
-        <v>445</v>
+        <v>361</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -6366,13 +6320,10 @@
         <v>155</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>363</v>
+        <v>432</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="H12" t="s">
-        <v>445</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -6380,13 +6331,10 @@
         <v>156</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>363</v>
+        <v>432</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="H13" t="s">
-        <v>445</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -6394,13 +6342,10 @@
         <v>157</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="H14" t="s">
-        <v>444</v>
+        <v>362</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -6408,13 +6353,10 @@
         <v>158</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="H15" t="s">
-        <v>444</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -6422,30 +6364,24 @@
         <v>159</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>363</v>
+        <v>432</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="H16" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>252</v>
       </c>
       <c r="B17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>263</v>
+        <v>393</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="H17" t="s">
-        <v>439</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -6457,7 +6393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -6467,7 +6403,7 @@
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" customWidth="1"/>
@@ -6478,13 +6414,13 @@
         <v>253</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>254</v>
@@ -6493,10 +6429,10 @@
         <v>255</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -6504,7 +6440,7 @@
         <v>160</v>
       </c>
       <c r="D2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6512,13 +6448,10 @@
         <v>161</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>256</v>
+        <v>437</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="H3" t="s">
-        <v>440</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -6526,10 +6459,10 @@
         <v>162</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6555,10 +6488,10 @@
         <v>164</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -6566,10 +6499,10 @@
         <v>165</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6599,10 +6532,10 @@
         <v>168</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -6610,13 +6543,10 @@
         <v>157</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>417</v>
+        <v>434</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="H12" t="s">
-        <v>444</v>
+        <v>362</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -6624,13 +6554,10 @@
         <v>169</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>363</v>
+        <v>432</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="H13" t="s">
-        <v>445</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -6638,17 +6565,14 @@
         <v>170</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>363</v>
+        <v>432</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="H14" t="s">
-        <v>445</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="22" t="s">
         <v>171</v>
       </c>
     </row>
@@ -6657,10 +6581,10 @@
         <v>252</v>
       </c>
       <c r="B16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>199</v>
@@ -6675,8 +6599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:F9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6685,7 +6609,7 @@
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="19.28515625" customWidth="1"/>
@@ -6696,13 +6620,13 @@
         <v>253</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>254</v>
@@ -6711,10 +6635,10 @@
         <v>255</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6722,7 +6646,7 @@
         <v>172</v>
       </c>
       <c r="D2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -6731,33 +6655,28 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
-      <c r="H3" t="s">
-        <v>446</v>
-      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>256</v>
+        <v>436</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>440</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="H4" s="21"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>175</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -6787,10 +6706,10 @@
         <v>176</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -6798,10 +6717,10 @@
         <v>177</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -6809,10 +6728,10 @@
         <v>178</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -6820,10 +6739,10 @@
         <v>179</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -6831,10 +6750,10 @@
         <v>180</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -6842,10 +6761,10 @@
         <v>181</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -6853,13 +6772,10 @@
         <v>182</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>363</v>
+        <v>432</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="H14" t="s">
-        <v>445</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -6867,13 +6783,10 @@
         <v>170</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>363</v>
+        <v>432</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="H15" t="s">
-        <v>445</v>
+        <v>361</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -6881,61 +6794,52 @@
         <v>169</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>363</v>
+        <v>432</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="H16" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>183</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>363</v>
+        <v>432</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="H17" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>252</v>
       </c>
       <c r="B18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>375</v>
+        <v>435</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="H19" t="s">
-        <v>446</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Labels, Definitionen, kleine Änderungen
nvto:hasSurtitleTranslator wieder rausgeworfen, zu speziell
nvto:PROPOSED_hasMember rausgeworfen
nvto:PROPOSED_hasPrompter (souffleur) eingeführt
nvto:PROPOSED_hasSeamster eingeführt
nvto:PROPOSED_hasPantomime eingeführt
nvto:PROPOSED_hasStageManager eingeführt
nvto:hasPlaywright zurück zu Proposed

nvto:PROPOSED_Festival -> nvto:Festival
nvto:PROPOSED_FestivalInstance -> nvto:FestivalEdition
nvto:PROPOSED_ArtisticDirector

nvto:hasLightDesigner -> nvto:hasLightingDesigner (auch in metapy)

Deutsche Labels, Definitionen und ggf Scope Notes für alle Klassen
Deutsche Labels für alle Properties
</commit_message>
<xml_diff>
--- a/Mapping/Mapping_Meta_Py.xlsx
+++ b/Mapping/Mapping_Meta_Py.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Dropbox\ITI\NVT_Data-Model\Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FAD21D-FFF2-4645-9FF3-74145C5508C8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9305149B-DDF3-4EEC-98B1-7DB0F4367773}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="927" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31920" yWindow="1965" windowWidth="15510" windowHeight="12540" tabRatio="927" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produktionen" sheetId="1" r:id="rId1"/>
@@ -717,9 +717,6 @@
     <t>has mask designer</t>
   </si>
   <si>
-    <t>nvto:hasLightDesigner</t>
-  </si>
-  <si>
     <t>has light designer</t>
   </si>
   <si>
@@ -1372,6 +1369,9 @@
   </si>
   <si>
     <t>has labeling</t>
+  </si>
+  <si>
+    <t>nvto:hasLightingDesigner</t>
   </si>
 </sst>
 </file>
@@ -1927,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,28 +1946,28 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1976,7 +1976,7 @@
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1986,7 +1986,7 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="11" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>198</v>
@@ -2025,7 +2025,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="H6" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2035,7 +2035,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="H7" s="10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2045,7 +2045,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="11" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>201</v>
@@ -2058,7 +2058,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="11" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>202</v>
@@ -2214,10 +2214,10 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="11" t="s">
+        <v>443</v>
+      </c>
+      <c r="F21" s="12" t="s">
         <v>225</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2227,7 +2227,7 @@
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>218</v>
@@ -2240,10 +2240,10 @@
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>228</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2253,10 +2253,10 @@
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>230</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2266,10 +2266,10 @@
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="F25" s="12" t="s">
         <v>232</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2279,10 +2279,10 @@
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2292,10 +2292,10 @@
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="F27" s="12" t="s">
         <v>236</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2305,10 +2305,10 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="H28" s="10" t="s">
         <v>418</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2318,7 +2318,7 @@
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="11" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>202</v>
@@ -2331,10 +2331,10 @@
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="F30" s="12" t="s">
         <v>238</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2344,10 +2344,10 @@
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>240</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2355,14 +2355,14 @@
         <v>30</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="F32" s="12" t="s">
         <v>244</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2370,14 +2370,14 @@
         <v>31</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="F33" s="12" t="s">
         <v>246</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2387,10 +2387,10 @@
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F34" s="12" t="s">
         <v>248</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2400,10 +2400,10 @@
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F35" s="12" t="s">
         <v>248</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2413,41 +2413,41 @@
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F36" s="12" t="s">
         <v>248</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E37" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="F37" s="12" t="s">
         <v>242</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>199</v>
@@ -2455,15 +2455,15 @@
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>200</v>
@@ -2495,28 +2495,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2524,7 +2524,7 @@
         <v>184</v>
       </c>
       <c r="D2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2532,13 +2532,13 @@
         <v>185</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H3" s="21"/>
     </row>
@@ -2549,7 +2549,7 @@
       <c r="E4" s="25"/>
       <c r="F4" s="3"/>
       <c r="H4" s="21" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2557,13 +2557,13 @@
         <v>187</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H5" s="21"/>
     </row>
@@ -2572,10 +2572,10 @@
         <v>188</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2583,10 +2583,10 @@
         <v>180</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>376</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2594,10 +2594,10 @@
         <v>181</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>378</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2605,10 +2605,10 @@
         <v>183</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -2637,28 +2637,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2666,7 +2666,7 @@
         <v>189</v>
       </c>
       <c r="D2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2674,13 +2674,13 @@
         <v>190</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H3" s="21"/>
     </row>
@@ -2691,7 +2691,7 @@
       <c r="E4" s="25"/>
       <c r="F4" s="3"/>
       <c r="H4" s="21" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2699,13 +2699,13 @@
         <v>192</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H5" s="21"/>
     </row>
@@ -2714,10 +2714,10 @@
         <v>180</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>376</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2725,10 +2725,10 @@
         <v>181</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>378</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2736,10 +2736,10 @@
         <v>183</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2772,25 +2772,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2798,7 +2798,7 @@
         <v>172</v>
       </c>
       <c r="D2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2806,10 +2806,10 @@
         <v>193</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H3" s="21"/>
     </row>
@@ -2825,10 +2825,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>199</v>
@@ -2857,25 +2857,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2883,7 +2883,7 @@
         <v>172</v>
       </c>
       <c r="D2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2891,10 +2891,10 @@
         <v>196</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H3" s="21"/>
     </row>
@@ -2912,10 +2912,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>199</v>
@@ -2948,28 +2948,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2977,7 +2977,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2985,10 +2985,10 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2996,7 +2996,7 @@
         <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>201</v>
@@ -3017,10 +3017,10 @@
         <v>37</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3028,10 +3028,10 @@
         <v>38</v>
       </c>
       <c r="E8" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>264</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3039,10 +3039,10 @@
         <v>39</v>
       </c>
       <c r="E9" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>264</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3050,10 +3050,10 @@
         <v>40</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3061,7 +3061,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>202</v>
@@ -3193,10 +3193,10 @@
         <v>19</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3204,7 +3204,7 @@
         <v>20</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>218</v>
@@ -3215,10 +3215,10 @@
         <v>21</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -3226,10 +3226,10 @@
         <v>22</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -3237,10 +3237,10 @@
         <v>23</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3248,10 +3248,10 @@
         <v>24</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3259,10 +3259,10 @@
         <v>25</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -3270,10 +3270,10 @@
         <v>41</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -3281,10 +3281,10 @@
         <v>42</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>267</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -3292,7 +3292,7 @@
         <v>27</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>202</v>
@@ -3303,12 +3303,12 @@
         <v>26</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3316,10 +3316,10 @@
         <v>43</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3327,13 +3327,13 @@
         <v>44</v>
       </c>
       <c r="C35" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E35" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3341,13 +3341,13 @@
         <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>246</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3355,10 +3355,10 @@
         <v>32</v>
       </c>
       <c r="E37" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3366,10 +3366,10 @@
         <v>33</v>
       </c>
       <c r="E38" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3377,41 +3377,41 @@
         <v>34</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>272</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B40" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="B41" t="s">
+        <v>259</v>
+      </c>
+      <c r="D41" t="s">
         <v>274</v>
       </c>
-      <c r="B41" t="s">
-        <v>260</v>
-      </c>
-      <c r="D41" t="s">
-        <v>275</v>
-      </c>
       <c r="E41" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>270</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -3441,28 +3441,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3470,10 +3470,10 @@
         <v>46</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3481,12 +3481,12 @@
         <v>47</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3494,7 +3494,7 @@
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3502,10 +3502,10 @@
         <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3513,10 +3513,10 @@
         <v>50</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3524,10 +3524,10 @@
         <v>51</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3535,10 +3535,10 @@
         <v>52</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3546,13 +3546,13 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3560,10 +3560,10 @@
         <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3571,10 +3571,10 @@
         <v>55</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -3582,10 +3582,10 @@
         <v>56</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -3593,10 +3593,10 @@
         <v>57</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -3604,10 +3604,10 @@
         <v>58</v>
       </c>
       <c r="E14" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="F14" s="17" t="s">
         <v>281</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -3615,10 +3615,10 @@
         <v>59</v>
       </c>
       <c r="E15" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="F15" s="17" t="s">
         <v>264</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -3626,10 +3626,10 @@
         <v>60</v>
       </c>
       <c r="E16" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="F16" s="17" t="s">
         <v>281</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3637,10 +3637,10 @@
         <v>61</v>
       </c>
       <c r="E17" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="F17" s="17" t="s">
         <v>264</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3648,7 +3648,7 @@
         <v>62</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>198</v>
@@ -3659,10 +3659,10 @@
         <v>63</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>283</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -3680,10 +3680,10 @@
         <v>66</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>285</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3691,10 +3691,10 @@
         <v>67</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3702,10 +3702,10 @@
         <v>68</v>
       </c>
       <c r="E24" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>289</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3713,10 +3713,10 @@
         <v>69</v>
       </c>
       <c r="E25" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>264</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -3724,10 +3724,10 @@
         <v>70</v>
       </c>
       <c r="E26" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>264</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -3735,10 +3735,10 @@
         <v>71</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>291</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3823,10 +3823,10 @@
         <v>19</v>
       </c>
       <c r="E35" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3834,7 +3834,7 @@
         <v>20</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>218</v>
@@ -3845,10 +3845,10 @@
         <v>21</v>
       </c>
       <c r="E37" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3856,10 +3856,10 @@
         <v>22</v>
       </c>
       <c r="E38" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3867,10 +3867,10 @@
         <v>23</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3889,10 +3889,10 @@
         <v>24</v>
       </c>
       <c r="E41" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3900,10 +3900,10 @@
         <v>25</v>
       </c>
       <c r="E42" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>236</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3911,7 +3911,7 @@
         <v>27</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>202</v>
@@ -3922,10 +3922,10 @@
         <v>74</v>
       </c>
       <c r="E44" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>293</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3933,10 +3933,10 @@
         <v>75</v>
       </c>
       <c r="E45" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>295</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3944,12 +3944,12 @@
         <v>26</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3957,10 +3957,10 @@
         <v>76</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3968,10 +3968,10 @@
         <v>77</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -3979,10 +3979,10 @@
         <v>78</v>
       </c>
       <c r="E49" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -3990,10 +3990,10 @@
         <v>33</v>
       </c>
       <c r="E50" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -4001,10 +4001,10 @@
         <v>34</v>
       </c>
       <c r="E51" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F51" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -4012,13 +4012,13 @@
         <v>79</v>
       </c>
       <c r="C52" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -4026,13 +4026,13 @@
         <v>80</v>
       </c>
       <c r="C53" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -4055,13 +4055,13 @@
         <v>84</v>
       </c>
       <c r="C57" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E57" t="s">
+        <v>441</v>
+      </c>
+      <c r="F57" t="s">
         <v>442</v>
-      </c>
-      <c r="F57" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -4069,13 +4069,13 @@
         <v>85</v>
       </c>
       <c r="C58" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -4083,10 +4083,10 @@
         <v>86</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -4094,7 +4094,7 @@
         <v>87</v>
       </c>
       <c r="C60" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E60" s="10"/>
     </row>
@@ -4110,7 +4110,7 @@
         <v>89</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F62" s="3"/>
     </row>
@@ -4119,13 +4119,13 @@
         <v>90</v>
       </c>
       <c r="C63" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E63" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -4133,13 +4133,13 @@
         <v>91</v>
       </c>
       <c r="C64" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -4147,13 +4147,13 @@
         <v>92</v>
       </c>
       <c r="C65" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -4161,13 +4161,13 @@
         <v>93</v>
       </c>
       <c r="C66" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -4175,21 +4175,21 @@
         <v>94</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H67" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B68" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>199</v>
@@ -4197,47 +4197,47 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B69" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C69" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E69" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B70" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D70" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="B71" t="s">
+        <v>259</v>
+      </c>
+      <c r="D71" t="s">
+        <v>317</v>
+      </c>
+      <c r="E71" s="18" t="s">
         <v>313</v>
-      </c>
-      <c r="B71" t="s">
-        <v>260</v>
-      </c>
-      <c r="D71" t="s">
-        <v>318</v>
-      </c>
-      <c r="E71" s="18" t="s">
-        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -4249,8 +4249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4267,28 +4267,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -4296,10 +4296,10 @@
         <v>46</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4307,12 +4307,12 @@
         <v>95</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4320,7 +4320,7 @@
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4328,10 +4328,10 @@
         <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4339,10 +4339,10 @@
         <v>50</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4350,10 +4350,10 @@
         <v>96</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4361,10 +4361,10 @@
         <v>52</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4372,13 +4372,13 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4386,10 +4386,10 @@
         <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4397,10 +4397,10 @@
         <v>97</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4408,10 +4408,10 @@
         <v>56</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4419,10 +4419,10 @@
         <v>98</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4430,10 +4430,10 @@
         <v>58</v>
       </c>
       <c r="E14" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="F14" s="17" t="s">
         <v>287</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4441,10 +4441,10 @@
         <v>59</v>
       </c>
       <c r="E15" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="F15" s="17" t="s">
         <v>319</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4452,10 +4452,10 @@
         <v>60</v>
       </c>
       <c r="E16" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="F16" s="17" t="s">
         <v>287</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4463,10 +4463,10 @@
         <v>61</v>
       </c>
       <c r="E17" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="F17" s="17" t="s">
         <v>319</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4474,7 +4474,7 @@
         <v>62</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>198</v>
@@ -4485,10 +4485,10 @@
         <v>63</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4506,10 +4506,10 @@
         <v>99</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4517,10 +4517,10 @@
         <v>100</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4528,10 +4528,10 @@
         <v>101</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4539,10 +4539,10 @@
         <v>102</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>291</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4561,10 +4561,10 @@
         <v>104</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>324</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4572,10 +4572,10 @@
         <v>105</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>326</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4583,10 +4583,10 @@
         <v>106</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>328</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4594,10 +4594,10 @@
         <v>107</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4605,7 +4605,7 @@
         <v>27</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>202</v>
@@ -4616,10 +4616,10 @@
         <v>108</v>
       </c>
       <c r="E32" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>319</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -4627,10 +4627,10 @@
         <v>109</v>
       </c>
       <c r="E33" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>319</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -4638,7 +4638,7 @@
         <v>110</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F34" s="3"/>
     </row>
@@ -4647,7 +4647,7 @@
         <v>111</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F35" s="3"/>
     </row>
@@ -4656,10 +4656,10 @@
         <v>112</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -4667,10 +4667,10 @@
         <v>113</v>
       </c>
       <c r="E37" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -4678,10 +4678,10 @@
         <v>114</v>
       </c>
       <c r="E38" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -4689,10 +4689,10 @@
         <v>115</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -4700,10 +4700,10 @@
         <v>116</v>
       </c>
       <c r="E40" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>337</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -4711,10 +4711,10 @@
         <v>117</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -4722,10 +4722,10 @@
         <v>34</v>
       </c>
       <c r="E42" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>337</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -4733,7 +4733,7 @@
         <v>118</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>201</v>
@@ -4744,7 +4744,7 @@
         <v>119</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>200</v>
@@ -4755,10 +4755,10 @@
         <v>120</v>
       </c>
       <c r="E45" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>339</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -4766,13 +4766,13 @@
         <v>79</v>
       </c>
       <c r="C46" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -4780,13 +4780,13 @@
         <v>85</v>
       </c>
       <c r="C47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -4794,10 +4794,10 @@
         <v>121</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H48" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -4812,13 +4812,13 @@
         <v>123</v>
       </c>
       <c r="C50" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -4846,7 +4846,7 @@
         <v>89</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F54" s="3"/>
     </row>
@@ -4855,13 +4855,13 @@
         <v>90</v>
       </c>
       <c r="C55" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E55" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F55" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -4869,13 +4869,13 @@
         <v>92</v>
       </c>
       <c r="C56" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E56" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F56" s="3" t="s">
         <v>341</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -4883,13 +4883,13 @@
         <v>93</v>
       </c>
       <c r="C57" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -4897,21 +4897,21 @@
         <v>94</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B59" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>199</v>
@@ -4919,47 +4919,47 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B60" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C60" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E60" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F60" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B61" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D61" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="B62" t="s">
+        <v>259</v>
+      </c>
+      <c r="D62" t="s">
+        <v>317</v>
+      </c>
+      <c r="E62" s="18" t="s">
         <v>313</v>
-      </c>
-      <c r="B62" t="s">
-        <v>260</v>
-      </c>
-      <c r="D62" t="s">
-        <v>318</v>
-      </c>
-      <c r="E62" s="18" t="s">
-        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -4990,28 +4990,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5019,10 +5019,10 @@
         <v>46</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5030,12 +5030,12 @@
         <v>47</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5043,7 +5043,7 @@
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5051,10 +5051,10 @@
         <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5062,16 +5062,16 @@
         <v>125</v>
       </c>
       <c r="C6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E6" t="s">
+        <v>441</v>
+      </c>
+      <c r="F6" t="s">
         <v>442</v>
       </c>
-      <c r="F6" t="s">
-        <v>443</v>
-      </c>
       <c r="H6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5079,10 +5079,10 @@
         <v>50</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5090,10 +5090,10 @@
         <v>51</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5101,10 +5101,10 @@
         <v>52</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5112,13 +5112,13 @@
         <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5126,10 +5126,10 @@
         <v>54</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5137,10 +5137,10 @@
         <v>97</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -5148,10 +5148,10 @@
         <v>56</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5159,10 +5159,10 @@
         <v>126</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -5170,10 +5170,10 @@
         <v>58</v>
       </c>
       <c r="E15" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="F15" s="17" t="s">
         <v>287</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5181,10 +5181,10 @@
         <v>59</v>
       </c>
       <c r="E16" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="F16" s="17" t="s">
         <v>319</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>320</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -5193,10 +5193,10 @@
         <v>60</v>
       </c>
       <c r="E17" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="F17" s="17" t="s">
         <v>287</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -5204,10 +5204,10 @@
         <v>61</v>
       </c>
       <c r="E18" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="F18" s="17" t="s">
         <v>319</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -5215,7 +5215,7 @@
         <v>127</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>198</v>
@@ -5236,10 +5236,10 @@
         <v>129</v>
       </c>
       <c r="E22" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -5247,10 +5247,10 @@
         <v>130</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -5258,10 +5258,10 @@
         <v>131</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -5269,10 +5269,10 @@
         <v>132</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -5280,10 +5280,10 @@
         <v>133</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -5291,10 +5291,10 @@
         <v>134</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -5302,10 +5302,10 @@
         <v>135</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -5313,13 +5313,13 @@
         <v>136</v>
       </c>
       <c r="C29" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -5327,13 +5327,13 @@
         <v>137</v>
       </c>
       <c r="C30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -5341,10 +5341,10 @@
         <v>138</v>
       </c>
       <c r="C31" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>199</v>
@@ -5355,13 +5355,13 @@
         <v>85</v>
       </c>
       <c r="C32" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -5369,10 +5369,10 @@
         <v>86</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -5380,10 +5380,10 @@
         <v>121</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H34" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -5391,13 +5391,13 @@
         <v>139</v>
       </c>
       <c r="C35" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -5405,10 +5405,10 @@
         <v>140</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -5416,13 +5416,13 @@
         <v>141</v>
       </c>
       <c r="C37" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -5443,7 +5443,7 @@
         <v>89</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F40" s="3"/>
     </row>
@@ -5452,13 +5452,13 @@
         <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E41" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -5466,13 +5466,13 @@
         <v>92</v>
       </c>
       <c r="C42" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E42" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>341</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -5480,13 +5480,13 @@
         <v>93</v>
       </c>
       <c r="C43" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -5494,23 +5494,23 @@
         <v>94</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
       <c r="H44" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B45" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>199</v>
@@ -5518,47 +5518,47 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B46" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C46" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E46" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B47" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D47" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="B48" t="s">
+        <v>259</v>
+      </c>
+      <c r="D48" t="s">
+        <v>317</v>
+      </c>
+      <c r="E48" s="18" t="s">
         <v>313</v>
-      </c>
-      <c r="B48" t="s">
-        <v>260</v>
-      </c>
-      <c r="D48" t="s">
-        <v>318</v>
-      </c>
-      <c r="E48" s="18" t="s">
-        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -5588,28 +5588,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5617,10 +5617,10 @@
         <v>46</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5628,12 +5628,12 @@
         <v>47</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5641,7 +5641,7 @@
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5649,10 +5649,10 @@
         <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5660,10 +5660,10 @@
         <v>50</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5671,10 +5671,10 @@
         <v>51</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5682,10 +5682,10 @@
         <v>52</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5693,13 +5693,13 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5707,10 +5707,10 @@
         <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5718,10 +5718,10 @@
         <v>142</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5729,10 +5729,10 @@
         <v>56</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -5740,10 +5740,10 @@
         <v>143</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5751,10 +5751,10 @@
         <v>58</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -5762,10 +5762,10 @@
         <v>59</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5773,10 +5773,10 @@
         <v>60</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -5784,10 +5784,10 @@
         <v>61</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -5795,7 +5795,7 @@
         <v>62</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>198</v>
@@ -5806,10 +5806,10 @@
         <v>63</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>283</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -5827,10 +5827,10 @@
         <v>68</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -5838,10 +5838,10 @@
         <v>69</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -5849,10 +5849,10 @@
         <v>144</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -5871,10 +5871,10 @@
         <v>70</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -5882,12 +5882,12 @@
         <v>26</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -5895,10 +5895,10 @@
         <v>76</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -5906,10 +5906,10 @@
         <v>77</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -5917,10 +5917,10 @@
         <v>78</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -5928,10 +5928,10 @@
         <v>33</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -5939,10 +5939,10 @@
         <v>34</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -5950,13 +5950,13 @@
         <v>146</v>
       </c>
       <c r="C33" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -5964,13 +5964,13 @@
         <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -5994,16 +5994,16 @@
         <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H38" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -6011,10 +6011,10 @@
         <v>86</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -6035,7 +6035,7 @@
         <v>89</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F42" s="3"/>
     </row>
@@ -6044,13 +6044,13 @@
         <v>90</v>
       </c>
       <c r="C43" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E43" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -6058,13 +6058,13 @@
         <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -6072,13 +6072,13 @@
         <v>92</v>
       </c>
       <c r="C45" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E45" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>341</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -6086,13 +6086,13 @@
         <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -6100,23 +6100,23 @@
         <v>94</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
       <c r="H47" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>199</v>
@@ -6124,47 +6124,47 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B49" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C49" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E49" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B50" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D50" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="B51" t="s">
+        <v>259</v>
+      </c>
+      <c r="D51" t="s">
+        <v>317</v>
+      </c>
+      <c r="E51" s="18" t="s">
         <v>313</v>
-      </c>
-      <c r="B51" t="s">
-        <v>260</v>
-      </c>
-      <c r="D51" t="s">
-        <v>318</v>
-      </c>
-      <c r="E51" s="18" t="s">
-        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -6193,28 +6193,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -6222,7 +6222,7 @@
         <v>147</v>
       </c>
       <c r="D2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6230,10 +6230,10 @@
         <v>148</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -6241,10 +6241,10 @@
         <v>149</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6252,10 +6252,10 @@
         <v>150</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6273,10 +6273,10 @@
         <v>151</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>357</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6284,10 +6284,10 @@
         <v>152</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>359</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -6295,13 +6295,13 @@
         <v>153</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -6309,10 +6309,10 @@
         <v>154</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -6320,10 +6320,10 @@
         <v>155</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -6331,10 +6331,10 @@
         <v>156</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -6342,10 +6342,10 @@
         <v>157</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -6353,10 +6353,10 @@
         <v>158</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -6364,24 +6364,24 @@
         <v>159</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -6411,28 +6411,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -6440,7 +6440,7 @@
         <v>160</v>
       </c>
       <c r="D2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6448,10 +6448,10 @@
         <v>161</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -6459,10 +6459,10 @@
         <v>162</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>363</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6488,10 +6488,10 @@
         <v>164</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>365</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -6499,10 +6499,10 @@
         <v>165</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>367</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6510,10 +6510,10 @@
         <v>166</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -6521,10 +6521,10 @@
         <v>167</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -6532,10 +6532,10 @@
         <v>168</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>369</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -6543,10 +6543,10 @@
         <v>157</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -6554,10 +6554,10 @@
         <v>169</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -6565,10 +6565,10 @@
         <v>170</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -6578,13 +6578,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>199</v>
@@ -6617,28 +6617,28 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="G1" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -6646,7 +6646,7 @@
         <v>172</v>
       </c>
       <c r="D2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -6661,10 +6661,10 @@
         <v>174</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H4" s="21"/>
     </row>
@@ -6673,10 +6673,10 @@
         <v>175</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>363</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -6706,10 +6706,10 @@
         <v>176</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>374</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -6717,10 +6717,10 @@
         <v>177</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -6728,10 +6728,10 @@
         <v>178</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -6739,10 +6739,10 @@
         <v>179</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -6750,10 +6750,10 @@
         <v>180</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>376</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -6761,10 +6761,10 @@
         <v>181</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>378</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -6772,10 +6772,10 @@
         <v>182</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -6783,10 +6783,10 @@
         <v>170</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -6794,10 +6794,10 @@
         <v>169</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -6805,21 +6805,21 @@
         <v>183</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>199</v>
@@ -6827,19 +6827,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E19" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>372</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>